<commit_message>
Updated the rubric for lab 3
</commit_message>
<xml_diff>
--- a/Labs/Lab03/Lab3Rubric_CS295N.xlsx
+++ b/Labs/Lab03/Lab3Rubric_CS295N.xlsx
@@ -1,32 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DataCard/Repos/CS295N-CourseMaterials/Labs/Lab03/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\birdb\Repos\CS295N_Repos\CS295N-CourseMaterials\Labs\Lab03\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EBBC8C8-3595-404D-8FC6-6BDEEBB66AC8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E47D22E-75A7-41E1-A3DC-8D62FAEC21E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2400" yWindow="500" windowWidth="12860" windowHeight="16520" activeTab="1" xr2:uid="{BBA0DDDD-2AF9-F84B-99D8-B3B03BF552D8}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11280" xr2:uid="{BBA0DDDD-2AF9-F84B-99D8-B3B03BF552D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Rubric" sheetId="1" r:id="rId1"/>
     <sheet name="Grade" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="25">
   <si>
     <t xml:space="preserve">Total: </t>
   </si>
@@ -98,6 +109,9 @@
   </si>
   <si>
     <t>Exercise completed--screenshot</t>
+  </si>
+  <si>
+    <t>PR sent to lab partner</t>
   </si>
 </sst>
 </file>
@@ -178,13 +192,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -204,9 +218,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -244,7 +258,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -350,7 +364,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -492,7 +506,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -502,14 +516,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB1F9B31-93F6-EA4C-88EB-610E0C385149}">
   <dimension ref="A1:C64"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11.1875" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="36" customWidth="1"/>
-    <col min="2" max="2" width="7.6640625" customWidth="1"/>
+    <col min="2" max="2" width="7.6875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -563,7 +577,7 @@
         <v>14</v>
       </c>
       <c r="B10">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -576,7 +590,7 @@
         <v>18</v>
       </c>
       <c r="B12">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -619,12 +633,20 @@
         <v>3</v>
       </c>
     </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19">
+        <v>3</v>
+      </c>
+    </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
         <v>5</v>
       </c>
       <c r="B20">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -735,17 +757,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{500450CF-4036-4C7A-B372-CF82A859E7EB}">
   <dimension ref="A1:E67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView topLeftCell="A15" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11.1875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="30.33203125" customWidth="1"/>
-    <col min="2" max="2" width="7.6640625" customWidth="1"/>
-    <col min="3" max="3" width="6.1640625" customWidth="1"/>
-    <col min="4" max="4" width="1.33203125" customWidth="1"/>
-    <col min="5" max="5" width="18.33203125" customWidth="1"/>
+    <col min="1" max="1" width="30.3125" customWidth="1"/>
+    <col min="2" max="2" width="7.6875" customWidth="1"/>
+    <col min="3" max="3" width="6.1875" customWidth="1"/>
+    <col min="4" max="4" width="1.3125" customWidth="1"/>
+    <col min="5" max="5" width="18.3125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -754,7 +776,7 @@
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:5" ht="34" customHeight="1">
+    <row r="2" spans="1:5" ht="34.049999999999997" customHeight="1">
       <c r="A2" s="7" t="s">
         <v>22</v>
       </c>
@@ -764,13 +786,13 @@
       <c r="E2" s="7"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
@@ -790,7 +812,7 @@
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="8"/>
+      <c r="E5" s="6"/>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
@@ -802,22 +824,22 @@
       <c r="C6">
         <v>10</v>
       </c>
-      <c r="E6" s="8"/>
+      <c r="E6" s="6"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="E7" s="8"/>
+      <c r="E7" s="6"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="8"/>
+      <c r="E8" s="6"/>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="8"/>
+      <c r="E9" s="6"/>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
@@ -829,37 +851,37 @@
       <c r="C10">
         <v>3</v>
       </c>
-      <c r="E10" s="8"/>
+      <c r="E10" s="6"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>14</v>
       </c>
       <c r="B11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C11">
-        <v>3</v>
-      </c>
-      <c r="E11" s="8"/>
+        <v>2</v>
+      </c>
+      <c r="E11" s="6"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="8"/>
+      <c r="E12" s="6"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>18</v>
       </c>
       <c r="B13">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C13">
-        <v>5</v>
-      </c>
-      <c r="E13" s="8"/>
+        <v>4</v>
+      </c>
+      <c r="E13" s="6"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
@@ -871,13 +893,13 @@
       <c r="C14">
         <v>4</v>
       </c>
-      <c r="E14" s="8"/>
+      <c r="E14" s="6"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E15" s="8"/>
+      <c r="E15" s="6"/>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
@@ -889,7 +911,7 @@
       <c r="C16">
         <v>2</v>
       </c>
-      <c r="E16" s="8"/>
+      <c r="E16" s="6"/>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
@@ -901,10 +923,10 @@
       <c r="C17">
         <v>5</v>
       </c>
-      <c r="E17" s="8"/>
+      <c r="E17" s="6"/>
     </row>
     <row r="18" spans="1:5">
-      <c r="E18" s="8"/>
+      <c r="E18" s="6"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
@@ -916,25 +938,34 @@
       <c r="C19">
         <v>3</v>
       </c>
-      <c r="E19" s="8"/>
+      <c r="E19" s="6"/>
     </row>
     <row r="20" spans="1:5">
-      <c r="E20" s="8"/>
+      <c r="A20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20">
+        <v>3</v>
+      </c>
+      <c r="C20">
+        <v>3</v>
+      </c>
+      <c r="E20" s="6"/>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>5</v>
       </c>
       <c r="B21">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C21">
-        <v>5</v>
-      </c>
-      <c r="E21" s="8"/>
+        <v>4</v>
+      </c>
+      <c r="E21" s="6"/>
     </row>
     <row r="22" spans="1:5">
-      <c r="E22" s="8"/>
+      <c r="E22" s="6"/>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="1" t="s">
@@ -948,7 +979,7 @@
         <f>SUM(C5:C21)</f>
         <v>40</v>
       </c>
-      <c r="E23" s="8"/>
+      <c r="E23" s="6"/>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="1"/>

</xml_diff>

<commit_message>
Updated the lab 3 rubric with the correct htm version and with comments in the xlsx
</commit_message>
<xml_diff>
--- a/Labs/Lab03/Lab3Rubric_CS295N.xlsx
+++ b/Labs/Lab03/Lab3Rubric_CS295N.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\birdb\Repos\CS295N_Repos\CS295N-CourseMaterials\Labs\Lab03\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E47D22E-75A7-41E1-A3DC-8D62FAEC21E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{84807FFC-1720-49C6-94A5-38F8A17191DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11280" xr2:uid="{BBA0DDDD-2AF9-F84B-99D8-B3B03BF552D8}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10995" windowHeight="11363" xr2:uid="{BBA0DDDD-2AF9-F84B-99D8-B3B03BF552D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Rubric" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="27">
   <si>
     <t xml:space="preserve">Total: </t>
   </si>
@@ -112,6 +112,12 @@
   </si>
   <si>
     <t>PR sent to lab partner</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Good</t>
   </si>
 </sst>
 </file>
@@ -516,7 +522,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB1F9B31-93F6-EA4C-88EB-610E0C385149}">
   <dimension ref="A1:C64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -757,8 +763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{500450CF-4036-4C7A-B372-CF82A859E7EB}">
   <dimension ref="A1:E67"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:B21"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1875" defaultRowHeight="15.75"/>
@@ -824,7 +830,9 @@
       <c r="C6">
         <v>10</v>
       </c>
-      <c r="E6" s="6"/>
+      <c r="E6" s="6" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="7" spans="1:5">
       <c r="E7" s="6"/>
@@ -851,7 +859,9 @@
       <c r="C10">
         <v>3</v>
       </c>
-      <c r="E10" s="6"/>
+      <c r="E10" s="6" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
@@ -863,7 +873,9 @@
       <c r="C11">
         <v>2</v>
       </c>
-      <c r="E11" s="6"/>
+      <c r="E11" s="6" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="2" t="s">
@@ -881,7 +893,9 @@
       <c r="C13">
         <v>4</v>
       </c>
-      <c r="E13" s="6"/>
+      <c r="E13" s="6" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
@@ -893,7 +907,9 @@
       <c r="C14">
         <v>4</v>
       </c>
-      <c r="E14" s="6"/>
+      <c r="E14" s="6" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="2" t="s">
@@ -911,7 +927,9 @@
       <c r="C16">
         <v>2</v>
       </c>
-      <c r="E16" s="6"/>
+      <c r="E16" s="6" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
@@ -923,7 +941,9 @@
       <c r="C17">
         <v>5</v>
       </c>
-      <c r="E17" s="6"/>
+      <c r="E17" s="6" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="18" spans="1:5">
       <c r="E18" s="6"/>
@@ -938,7 +958,9 @@
       <c r="C19">
         <v>3</v>
       </c>
-      <c r="E19" s="6"/>
+      <c r="E19" s="6" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
@@ -950,7 +972,9 @@
       <c r="C20">
         <v>3</v>
       </c>
-      <c r="E20" s="6"/>
+      <c r="E20" s="6" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
@@ -962,7 +986,9 @@
       <c r="C21">
         <v>4</v>
       </c>
-      <c r="E21" s="6"/>
+      <c r="E21" s="6" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="22" spans="1:5">
       <c r="E22" s="6"/>

</xml_diff>

<commit_message>
Yet another update to the lab 3 rubric
</commit_message>
<xml_diff>
--- a/Labs/Lab03/Lab3Rubric_CS295N.xlsx
+++ b/Labs/Lab03/Lab3Rubric_CS295N.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\birdb\Repos\CS295N_Repos\CS295N-CourseMaterials\Labs\Lab03\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{84807FFC-1720-49C6-94A5-38F8A17191DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{94A90B38-59DC-4DF9-8803-88AD59A967DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="10995" windowHeight="11363" xr2:uid="{BBA0DDDD-2AF9-F84B-99D8-B3B03BF552D8}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="28">
   <si>
     <t xml:space="preserve">Total: </t>
   </si>
@@ -81,9 +81,6 @@
     <t>2 or more model classes</t>
   </si>
   <si>
-    <t>5 model properties minimum</t>
-  </si>
-  <si>
     <t>Models</t>
   </si>
   <si>
@@ -96,9 +93,6 @@
     <t>form for entering msg, story, or post</t>
   </si>
   <si>
-    <t>HTTP Post method to echo entry</t>
-  </si>
-  <si>
     <t>Lab 3 Rubric for All Groups</t>
   </si>
   <si>
@@ -118,6 +112,15 @@
   </si>
   <si>
     <t>Good</t>
+  </si>
+  <si>
+    <t>&gt;= 5 properties including Date, AppUser and an int</t>
+  </si>
+  <si>
+    <t>HTTP Post method to add date and echo entry</t>
+  </si>
+  <si>
+    <t>Points</t>
   </si>
 </sst>
 </file>
@@ -190,7 +193,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -205,6 +208,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -522,19 +528,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB1F9B31-93F6-EA4C-88EB-610E0C385149}">
   <dimension ref="A1:C64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="36" customWidth="1"/>
-    <col min="2" max="2" width="7.6875" customWidth="1"/>
+    <col min="1" max="1" width="42.375" customWidth="1"/>
+    <col min="2" max="2" width="6.0625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B1" s="1"/>
     </row>
@@ -543,7 +549,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="C3" s="1"/>
     </row>
@@ -567,7 +573,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -578,22 +584,22 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
-        <v>14</v>
+    <row r="10" spans="1:3" ht="31.5">
+      <c r="A10" s="9" t="s">
+        <v>25</v>
       </c>
       <c r="B10">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B12">
         <v>4</v>
@@ -609,7 +615,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -620,12 +626,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
-      <c r="A16" t="s">
-        <v>19</v>
+    <row r="16" spans="1:3" ht="31.5">
+      <c r="A16" s="9" t="s">
+        <v>26</v>
       </c>
       <c r="B16">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -641,7 +647,7 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B19">
         <v>3</v>
@@ -763,8 +769,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{500450CF-4036-4C7A-B372-CF82A859E7EB}">
   <dimension ref="A1:E67"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView topLeftCell="A5" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1875" defaultRowHeight="15.75"/>
@@ -784,7 +790,7 @@
     </row>
     <row r="2" spans="1:5" ht="34.049999999999997" customHeight="1">
       <c r="A2" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -811,7 +817,7 @@
         <v>2</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -822,7 +828,7 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B6">
         <v>10</v>
@@ -831,7 +837,7 @@
         <v>10</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -845,7 +851,7 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E9" s="6"/>
     </row>
@@ -860,32 +866,32 @@
         <v>3</v>
       </c>
       <c r="E10" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="31.5">
+      <c r="A11" s="9" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" t="s">
-        <v>14</v>
-      </c>
       <c r="B11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E12" s="6"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13">
         <v>4</v>
@@ -894,7 +900,7 @@
         <v>4</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -908,12 +914,12 @@
         <v>4</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E15" s="6"/>
     </row>
@@ -928,21 +934,21 @@
         <v>2</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" t="s">
-        <v>19</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="31.5">
+      <c r="A17" s="9" t="s">
+        <v>26</v>
       </c>
       <c r="B17">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C17">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -959,12 +965,12 @@
         <v>3</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B20">
         <v>3</v>
@@ -973,7 +979,7 @@
         <v>3</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -987,7 +993,7 @@
         <v>4</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:5">

</xml_diff>